<commit_message>
Added list table and error handling
</commit_message>
<xml_diff>
--- a/data/GiffordGunLawStrength.xlsx
+++ b/data/GiffordGunLawStrength.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\missm\source\repos\MichelleRobertsBU\Gun-Law-Effects-on-Homicides-by-Firearms\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AAB9994-600C-47AF-8CA7-F35A52CD4B92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4F2AFF-E6EA-49D5-9340-CDF13931711B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10404" yWindow="720" windowWidth="12012" windowHeight="10992" xr2:uid="{BDB16AB1-F335-404F-8B22-D44F29487647}"/>
   </bookViews>
@@ -233,7 +233,7 @@
     <t>Death_Rank</t>
   </si>
   <si>
-    <t>Rate_per_100K</t>
+    <t>Rate_per_Hundred</t>
   </si>
 </sst>
 </file>
@@ -658,7 +658,7 @@
   <dimension ref="A1:E52"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>